<commit_message>
Subindo alterações e testes
</commit_message>
<xml_diff>
--- a/relatorio_fap.xlsx
+++ b/relatorio_fap.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -471,47 +471,611 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
+          <t>53.458.313</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>3L SERVICOS LTDA</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>53.458.313/0001-54</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>53.458.313/0001-54</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>GO</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>GOIANIA</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>2025</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>1,0000</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>30/10/2025 19:55:19</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
           <t>02.618.143</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
+      <c r="B3" t="inlineStr">
         <is>
           <t>A IDEAL SOLUCOES ANTICORROSIVAS LTDA</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
+      <c r="C3" t="inlineStr">
         <is>
           <t>02.618.143/0001-97</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
+      <c r="D3" t="inlineStr">
         <is>
           <t>02.618.143/0001-97</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>R DAS ANGELICAS 309 QUADRA07 LOTE 14 15 16 17, PRQ OESTE INDUSTRIAL, GOIANIA - GO CEP: 74.375-440</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>R DAS ANGELICAS 309 QUADRA07 LOTE 14 15 16 17, PRQ OESTE INDUSTRIAL, GOIANIA - GO CEP: 74.375-440</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>2025</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>GO</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>GOIANIA</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>2025</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
         <is>
           <t>0,5000</t>
         </is>
       </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>29/10/2025 16:53:22</t>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>30/10/2025 19:55:41</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>43.228.913</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>ACADEMIA DE VENDAS LTDA</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>43.228.913/0001-72</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>43.228.913/0001-72</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>GO</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>GOIANIA</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>2025</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>1,0000</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>30/10/2025 19:56:02</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>03.720.943</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>ACP AGROPECUARIA LTDA</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>03.720.943/0001-87</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>03.720.943/0001-87</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>GO</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>CAMPOS VERDES</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>2025</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>1,0000</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>30/10/2025 19:56:25</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>03.720.943</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>ACP AGROPECUARIA LTDA</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>03.720.943/0003-49</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>03.720.943/0003-49</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>TO</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>PIUM</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>2025</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>1,0000</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>30/10/2025 19:56:37</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>03.720.943</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>ACP AGROPECUARIA LTDA</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>03.720.943/0007-72</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>03.720.943/0007-72</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>TO</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>PORTO NACIONAL</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>2025</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>0,5000</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>30/10/2025 19:56:49</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>03.720.943</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>ACP AGROPECUARIA LTDA</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>03.720.943/0011-59</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>03.720.943/0011-59</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>MT</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>PONTE BRANCA</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>2025</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>0,5000</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>30/10/2025 19:57:01</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>03.720.943</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>ACP AGROPECUARIA LTDA</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>03.720.943/0012-30</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>03.720.943/0012-30</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>GO</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>GOIANIA</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>2025</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>1,0000</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>30/10/2025 19:57:13</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>05.851.583</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>ACP PARTICIPACOES S A</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>05.851.583/0001-88</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>05.851.583/0001-88</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>GO</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>GOIANIA</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>2025</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>0,5000</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>30/10/2025 19:57:34</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>08.811.370</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>ACREFORT INDUSTRIA E COMERCIO DE RACOES LTDA</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>08.811.370/0001-10</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>08.811.370/0001-10</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>MT</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>PRIMAVERA DO LESTE</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>2025</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>0,5000</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>30/10/2025 19:57:56</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>08.811.370</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>ACREFORT INDUSTRIA E COMERCIO DE RACOES LTDA</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>08.811.370/0002-00</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>08.811.370/0002-00</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>MT</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>PRIMAVERA DO LESTE</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>2025</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>0,5000</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>30/10/2025 19:58:08</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>05.616.807</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>ACRESUL INDUSTRIA E COMERCIO LTDA</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>05.616.807/0001-77</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>05.616.807/0001-77</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>GO</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>ACREUNA</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>2025</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>0,5000</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>30/10/2025 19:58:30</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>37.181.936</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>AGB DISTRIBUIDORA DE ARMAS E MUNICOES S A</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>37.181.936/0001-76</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>37.181.936/0001-76</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>GO</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>ANAPOLIS</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>2025</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>0,5000</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>30/10/2025 19:58:52</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Commitando as últimas alterações da automação
</commit_message>
<xml_diff>
--- a/relatorio_fap.xlsx
+++ b/relatorio_fap.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I14"/>
+  <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -439,30 +439,25 @@
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>Estab_Nome</t>
+          <t>UF</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>UF</t>
+          <t>Municipio</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>Municipio</t>
+          <t>Vigencia</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>Vigencia</t>
+          <t>Aliquota</t>
         </is>
       </c>
       <c r="H1" t="inlineStr">
-        <is>
-          <t>Aliquota</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
         <is>
           <t>Data_Consulta</t>
         </is>
@@ -471,7 +466,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>53.458.313</t>
+          <t>53458313</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -481,44 +476,39 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>53.458.313/0001-54</t>
+          <t>53458313000154</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>53.458.313/0001-54</t>
+          <t>GO</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>GO</t>
+          <t>GOIANIA</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>GOIANIA</t>
+          <t>2025</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>2025</t>
+          <t>1,0000</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>1,0000</t>
-        </is>
-      </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>30/10/2025 19:55:19</t>
+          <t>31/10/2025 10:36:13</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>02.618.143</t>
+          <t>02618143</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -528,44 +518,39 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>02.618.143/0001-97</t>
+          <t>02618143000197</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>02.618.143/0001-97</t>
+          <t>GO</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>GO</t>
+          <t>GOIANIA</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>GOIANIA</t>
+          <t>2025</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>2025</t>
+          <t>0,5000</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>0,5000</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>30/10/2025 19:55:41</t>
+          <t>31/10/2025 10:36:36</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>43.228.913</t>
+          <t>43228913</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -575,44 +560,39 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>43.228.913/0001-72</t>
+          <t>43228913000172</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>43.228.913/0001-72</t>
+          <t>GO</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>GO</t>
+          <t>GOIANIA</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>GOIANIA</t>
+          <t>2025</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>2025</t>
+          <t>1,0000</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>1,0000</t>
-        </is>
-      </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>30/10/2025 19:56:02</t>
+          <t>31/10/2025 10:36:59</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>03.720.943</t>
+          <t>03720943</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -622,44 +602,39 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>03.720.943/0001-87</t>
+          <t>03720943000187</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>03.720.943/0001-87</t>
+          <t>GO</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>GO</t>
+          <t>CAMPOS VERDES</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>CAMPOS VERDES</t>
+          <t>2025</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>2025</t>
+          <t>1,0000</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>1,0000</t>
-        </is>
-      </c>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>30/10/2025 19:56:25</t>
+          <t>31/10/2025 10:37:23</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>03.720.943</t>
+          <t>03720943</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -669,44 +644,39 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>03.720.943/0003-49</t>
+          <t>03720943000349</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>03.720.943/0003-49</t>
+          <t>TO</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>TO</t>
+          <t>PIUM</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>PIUM</t>
+          <t>2025</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>2025</t>
+          <t>1,0000</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>1,0000</t>
-        </is>
-      </c>
-      <c r="I6" t="inlineStr">
-        <is>
-          <t>30/10/2025 19:56:37</t>
+          <t>31/10/2025 10:37:36</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>03.720.943</t>
+          <t>03720943</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -716,44 +686,39 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>03.720.943/0007-72</t>
+          <t>03720943000772</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>03.720.943/0007-72</t>
+          <t>TO</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>TO</t>
+          <t>PORTO NACIONAL</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>PORTO NACIONAL</t>
+          <t>2025</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>2025</t>
+          <t>0,5000</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>0,5000</t>
-        </is>
-      </c>
-      <c r="I7" t="inlineStr">
-        <is>
-          <t>30/10/2025 19:56:49</t>
+          <t>31/10/2025 10:37:48</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>03.720.943</t>
+          <t>03720943</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -763,44 +728,39 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>03.720.943/0011-59</t>
+          <t>03720943001159</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>03.720.943/0011-59</t>
+          <t>MT</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>MT</t>
+          <t>PONTE BRANCA</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>PONTE BRANCA</t>
+          <t>2025</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>2025</t>
+          <t>0,5000</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>0,5000</t>
-        </is>
-      </c>
-      <c r="I8" t="inlineStr">
-        <is>
-          <t>30/10/2025 19:57:01</t>
+          <t>31/10/2025 10:38:00</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>03.720.943</t>
+          <t>03720943</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -810,44 +770,39 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>03.720.943/0012-30</t>
+          <t>03720943001230</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>03.720.943/0012-30</t>
+          <t>GO</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>GO</t>
+          <t>GOIANIA</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>GOIANIA</t>
+          <t>2025</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>2025</t>
+          <t>1,0000</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>1,0000</t>
-        </is>
-      </c>
-      <c r="I9" t="inlineStr">
-        <is>
-          <t>30/10/2025 19:57:13</t>
+          <t>31/10/2025 10:38:13</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>05.851.583</t>
+          <t>05851583</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -857,44 +812,39 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>05.851.583/0001-88</t>
+          <t>05851583000188</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>05.851.583/0001-88</t>
+          <t>GO</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>GO</t>
+          <t>GOIANIA</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>GOIANIA</t>
+          <t>2025</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>2025</t>
+          <t>0,5000</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>0,5000</t>
-        </is>
-      </c>
-      <c r="I10" t="inlineStr">
-        <is>
-          <t>30/10/2025 19:57:34</t>
+          <t>31/10/2025 10:38:35</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>08.811.370</t>
+          <t>08811370</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -904,44 +854,39 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>08.811.370/0001-10</t>
+          <t>08811370000110</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>08.811.370/0001-10</t>
+          <t>MT</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>MT</t>
+          <t>PRIMAVERA DO LESTE</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>PRIMAVERA DO LESTE</t>
+          <t>2025</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>2025</t>
+          <t>0,5000</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>0,5000</t>
-        </is>
-      </c>
-      <c r="I11" t="inlineStr">
-        <is>
-          <t>30/10/2025 19:57:56</t>
+          <t>31/10/2025 10:38:59</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>08.811.370</t>
+          <t>08811370</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -951,44 +896,39 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>08.811.370/0002-00</t>
+          <t>08811370000200</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>08.811.370/0002-00</t>
+          <t>MT</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>MT</t>
+          <t>PRIMAVERA DO LESTE</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>PRIMAVERA DO LESTE</t>
+          <t>2025</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>2025</t>
+          <t>0,5000</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>0,5000</t>
-        </is>
-      </c>
-      <c r="I12" t="inlineStr">
-        <is>
-          <t>30/10/2025 19:58:08</t>
+          <t>31/10/2025 10:39:12</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>05.616.807</t>
+          <t>05616807</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -998,44 +938,39 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>05.616.807/0001-77</t>
+          <t>05616807000177</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>05.616.807/0001-77</t>
+          <t>GO</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>GO</t>
+          <t>ACREUNA</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>ACREUNA</t>
+          <t>2025</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>2025</t>
+          <t>0,5000</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>0,5000</t>
-        </is>
-      </c>
-      <c r="I13" t="inlineStr">
-        <is>
-          <t>30/10/2025 19:58:30</t>
+          <t>31/10/2025 10:39:35</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>37.181.936</t>
+          <t>37181936</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -1045,37 +980,116 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>37.181.936/0001-76</t>
+          <t>37181936000176</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>37.181.936/0001-76</t>
+          <t>GO</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
+          <t>ANAPOLIS</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>2025</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>0,5000</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>31/10/2025 10:39:58</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>37181936</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>AGB DISTRIBUIDORA DE ARMAS E MUNICOES S A</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>37181936000257</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>DF</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>BRASILIA</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>2025</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>1,0000</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>31/10/2025 10:40:11</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>07603106</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>AGNUS DEI ARTIGOS RELIGIOSOS LTDA</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>07603106000129</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
           <t>GO</t>
         </is>
       </c>
-      <c r="F14" t="inlineStr">
-        <is>
-          <t>ANAPOLIS</t>
-        </is>
-      </c>
-      <c r="G14" t="inlineStr">
-        <is>
-          <t>2025</t>
-        </is>
-      </c>
-      <c r="H14" t="inlineStr">
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>GOIANIA</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>2025</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
         <is>
           <t>0,5000</t>
         </is>
       </c>
-      <c r="I14" t="inlineStr">
-        <is>
-          <t>30/10/2025 19:58:52</t>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>31/10/2025 10:40:33</t>
         </is>
       </c>
     </row>

</xml_diff>